<commit_message>
FIX: Wite model by modelx v0.11.0 to fix PurePath error
</commit_message>
<xml_diff>
--- a/lifelib/projects/simplelife/model/Input/input.xlsx
+++ b/lifelib/projects/simplelife/model/Input/input.xlsx
@@ -360,74 +360,6 @@
     <cellStyle name="パーセント" xfId="2" builtinId="5"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 

</xml_diff>